<commit_message>
More work on lua support, improved interface lua access and added interface callbacks
</commit_message>
<xml_diff>
--- a/build/docs/lua.xlsx
+++ b/build/docs/lua.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Util" sheetId="1" r:id="rId1"/>
+    <sheet name="Game" sheetId="4" r:id="rId2"/>
+    <sheet name="Interface" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>function</t>
   </si>
@@ -36,18 +38,431 @@
     <t>prints text to the console</t>
   </si>
   <si>
-    <t>string msg</t>
-  </si>
-  <si>
     <t>both</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>includes a lua file to be executed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>relpath</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>msg</t>
+    </r>
+  </si>
+  <si>
+    <t>function (Game object)</t>
+  </si>
+  <si>
+    <t>GetResolution</t>
+  </si>
+  <si>
+    <t>returns the game resolution in a table {x,y}</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>returns true if fullscreen</t>
+  </si>
+  <si>
+    <t>IsFullscreen</t>
+  </si>
+  <si>
+    <t>GetFieldOfView</t>
+  </si>
+  <si>
+    <t>returns the field of view</t>
+  </si>
+  <si>
+    <t>SetFieldOfView</t>
+  </si>
+  <si>
+    <t>sets the field of view</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fov</t>
+    </r>
+  </si>
+  <si>
+    <t>SetFullscreen</t>
+  </si>
+  <si>
+    <t>sets the fullscreen state</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bool </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fullscreen</t>
+    </r>
+  </si>
+  <si>
+    <t>function (Interface object)</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">returns a new interface object of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+  </si>
+  <si>
+    <t>SetPosition</t>
+  </si>
+  <si>
+    <t>sets the interfaces position</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, [Interface </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>SetSize</t>
+  </si>
+  <si>
+    <t>sets the interfaces size</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xrel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yrel</t>
+    </r>
+  </si>
+  <si>
+    <t>SetBackground</t>
+  </si>
+  <si>
+    <t>sets the background color</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, float</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> g</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, float </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <t>SetVisible</t>
+  </si>
+  <si>
+    <t>sets if the control and children are rendered</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bool </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visible</t>
+    </r>
+  </si>
+  <si>
+    <t>SetText</t>
+  </si>
+  <si>
+    <t>sets the controls text</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>text</t>
+    </r>
+  </si>
+  <si>
+    <t>Activate</t>
+  </si>
+  <si>
+    <t>activates the interface object</t>
+  </si>
+  <si>
+    <t>GetFrameTime</t>
+  </si>
+  <si>
+    <t>returns the length of the previous frame (double)</t>
+  </si>
+  <si>
+    <t>RegisterEvent</t>
+  </si>
+  <si>
+    <t>registers and event, event name case sensitive</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, function </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>callback</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -400,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,18 +851,286 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -459,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Work converting chunk loading to a multihreaded process. Still needs work on loading new chunks with camera movement. Added position to debug pane
</commit_message>
<xml_diff>
--- a/build/docs/lua.xlsx
+++ b/build/docs/lua.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothy\Source\Repos\IsostratGame\build\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="22992" windowHeight="10548" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Util" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>function</t>
   </si>
@@ -447,12 +452,24 @@
       </rPr>
       <t>callback</t>
     </r>
+  </si>
+  <si>
+    <t>GetWireframeMode</t>
+  </si>
+  <si>
+    <t>gets the wireframe mode (solid=0, wireframe=1, wireframeui=2)</t>
+  </si>
+  <si>
+    <t>GetCameraPosition</t>
+  </si>
+  <si>
+    <t>gets the position of the camera (vector x,y,z)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,6 +541,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -571,7 +591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,9 +624,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,6 +676,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -814,22 +868,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -857,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -878,22 +932,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -907,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -918,7 +972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -929,7 +983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -943,7 +997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -954,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -968,7 +1022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -976,6 +1030,28 @@
         <v>46</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -986,22 +1062,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1029,7 +1105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1057,7 +1133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1085,7 +1161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1099,7 +1175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1110,7 +1186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1131,24 +1207,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>